<commit_message>
20230222 se modifica el excel ccon base a informacion correcta de la carrera 110 computacion
</commit_message>
<xml_diff>
--- a/Asignaturas Ingenieria.xlsx
+++ b/Asignaturas Ingenieria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djanr\Desktop\GitHubProjectsLocal\unam.fi.asignaturas\unam.fi.asignaturas.documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7F4247-B71C-4092-8EB6-1B1F526C0903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F538FD-B3B3-4EEF-8334-F7C4D72C6B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todas" sheetId="30" r:id="rId1"/>
@@ -3323,9 +3323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD65C8-55A5-4DB0-9D30-AE602BDAC74B}">
   <dimension ref="A1:P1434"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A709" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E758" sqref="E758"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8555,10 +8555,10 @@
         <v>285</v>
       </c>
       <c r="F151">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G151">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H151">
         <v>4</v>
@@ -9139,7 +9139,7 @@
         <v>7</v>
       </c>
       <c r="I168">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L168" t="s">
         <v>533</v>
@@ -9498,10 +9498,10 @@
         <v>308</v>
       </c>
       <c r="F179">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G179">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H179">
         <v>10</v>
@@ -50960,6 +50960,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B960:B1060"/>
+    <mergeCell ref="A839:A1060"/>
+    <mergeCell ref="B1061:B1187"/>
+    <mergeCell ref="B1188:B1306"/>
+    <mergeCell ref="B1307:B1434"/>
+    <mergeCell ref="A1061:A1434"/>
+    <mergeCell ref="B839:B959"/>
+    <mergeCell ref="B501:B619"/>
+    <mergeCell ref="B620:B693"/>
+    <mergeCell ref="B694:B764"/>
+    <mergeCell ref="B765:B838"/>
+    <mergeCell ref="A501:A838"/>
     <mergeCell ref="B430:B500"/>
     <mergeCell ref="A319:A500"/>
     <mergeCell ref="B2:B131"/>
@@ -50967,18 +50979,6 @@
     <mergeCell ref="B220:B318"/>
     <mergeCell ref="A2:A318"/>
     <mergeCell ref="B319:B429"/>
-    <mergeCell ref="B501:B619"/>
-    <mergeCell ref="B620:B693"/>
-    <mergeCell ref="B694:B764"/>
-    <mergeCell ref="B765:B838"/>
-    <mergeCell ref="A501:A838"/>
-    <mergeCell ref="B960:B1060"/>
-    <mergeCell ref="A839:A1060"/>
-    <mergeCell ref="B1061:B1187"/>
-    <mergeCell ref="B1188:B1306"/>
-    <mergeCell ref="B1307:B1434"/>
-    <mergeCell ref="A1061:A1434"/>
-    <mergeCell ref="B839:B959"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -81735,7 +81735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECB2A1A-C6A2-4DB4-AC88-C5C01CD8158F}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
@@ -88345,8 +88345,8 @@
   <dimension ref="A1:N89"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q75" sqref="Q75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -89579,7 +89579,7 @@
         <v>7</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J38" t="s">
         <v>533</v>

</xml_diff>

<commit_message>
20230312Se corrigen algunas asignaturas de carrera 109
</commit_message>
<xml_diff>
--- a/Asignaturas Ingenieria.xlsx
+++ b/Asignaturas Ingenieria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djanr\Desktop\GitHubProjectsLocal\unam.fi.asignaturas\unam.fi.asignaturas.documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3D728A-0A4D-4F8A-91F1-785291CD7BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF064AA-4C84-4340-BC2A-C5B9F564B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todas" sheetId="30" r:id="rId1"/>
@@ -3323,9 +3323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD65C8-55A5-4DB0-9D30-AE602BDAC74B}">
   <dimension ref="A1:P1434"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E194" sqref="E194"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5035,7 +5035,7 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H50">
         <v>10</v>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H51">
         <v>10</v>
@@ -5103,7 +5103,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H52">
         <v>10</v>
@@ -50960,6 +50960,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B960:B1060"/>
+    <mergeCell ref="A839:A1060"/>
+    <mergeCell ref="B1061:B1187"/>
+    <mergeCell ref="B1188:B1306"/>
+    <mergeCell ref="B1307:B1434"/>
+    <mergeCell ref="A1061:A1434"/>
+    <mergeCell ref="B839:B959"/>
+    <mergeCell ref="B501:B619"/>
+    <mergeCell ref="B620:B693"/>
+    <mergeCell ref="B694:B764"/>
+    <mergeCell ref="B765:B838"/>
+    <mergeCell ref="A501:A838"/>
     <mergeCell ref="B430:B500"/>
     <mergeCell ref="A319:A500"/>
     <mergeCell ref="B2:B131"/>
@@ -50967,18 +50979,6 @@
     <mergeCell ref="B220:B318"/>
     <mergeCell ref="A2:A318"/>
     <mergeCell ref="B319:B429"/>
-    <mergeCell ref="B501:B619"/>
-    <mergeCell ref="B620:B693"/>
-    <mergeCell ref="B694:B764"/>
-    <mergeCell ref="B765:B838"/>
-    <mergeCell ref="A501:A838"/>
-    <mergeCell ref="B960:B1060"/>
-    <mergeCell ref="A839:A1060"/>
-    <mergeCell ref="B1061:B1187"/>
-    <mergeCell ref="B1188:B1306"/>
-    <mergeCell ref="B1307:B1434"/>
-    <mergeCell ref="A1061:A1434"/>
-    <mergeCell ref="B839:B959"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -84031,8 +84031,8 @@
   <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R107" sqref="R107"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85641,7 +85641,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50">
         <v>10</v>
@@ -85673,7 +85673,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51">
         <v>10</v>
@@ -85705,7 +85705,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52">
         <v>10</v>
@@ -88344,8 +88344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAD1897-70C5-4597-AFFD-E842ACCFC6F5}">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
20230312 se modifican asignaturas de carrera 111
</commit_message>
<xml_diff>
--- a/Asignaturas Ingenieria.xlsx
+++ b/Asignaturas Ingenieria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djanr\Desktop\GitHubProjectsLocal\unam.fi.asignaturas\unam.fi.asignaturas.documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF064AA-4C84-4340-BC2A-C5B9F564B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162B8C4F-2114-4485-B95D-6F1E4D56277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todas" sheetId="30" r:id="rId1"/>
@@ -3323,9 +3323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BD65C8-55A5-4DB0-9D30-AE602BDAC74B}">
   <dimension ref="A1:P1434"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G235" sqref="G235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11348,10 +11348,10 @@
         <v>285</v>
       </c>
       <c r="F233">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G233">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H233">
         <v>3</v>
@@ -11419,7 +11419,7 @@
         <v>4</v>
       </c>
       <c r="G235">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H235">
         <v>3</v>
@@ -50960,6 +50960,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B430:B500"/>
+    <mergeCell ref="A319:A500"/>
+    <mergeCell ref="B2:B131"/>
+    <mergeCell ref="B132:B219"/>
+    <mergeCell ref="B220:B318"/>
+    <mergeCell ref="A2:A318"/>
+    <mergeCell ref="B319:B429"/>
+    <mergeCell ref="B501:B619"/>
+    <mergeCell ref="B620:B693"/>
+    <mergeCell ref="B694:B764"/>
+    <mergeCell ref="B765:B838"/>
+    <mergeCell ref="A501:A838"/>
     <mergeCell ref="B960:B1060"/>
     <mergeCell ref="A839:A1060"/>
     <mergeCell ref="B1061:B1187"/>
@@ -50967,18 +50979,6 @@
     <mergeCell ref="B1307:B1434"/>
     <mergeCell ref="A1061:A1434"/>
     <mergeCell ref="B839:B959"/>
-    <mergeCell ref="B501:B619"/>
-    <mergeCell ref="B620:B693"/>
-    <mergeCell ref="B694:B764"/>
-    <mergeCell ref="B765:B838"/>
-    <mergeCell ref="A501:A838"/>
-    <mergeCell ref="B430:B500"/>
-    <mergeCell ref="A319:A500"/>
-    <mergeCell ref="B2:B131"/>
-    <mergeCell ref="B132:B219"/>
-    <mergeCell ref="B220:B318"/>
-    <mergeCell ref="A2:A318"/>
-    <mergeCell ref="B319:B429"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -91239,9 +91239,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E72DC73-2456-4B9B-BC4C-6F7698CD869E}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N92" sqref="N92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -91727,10 +91727,10 @@
         <v>285</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -91794,7 +91794,7 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>3</v>

</xml_diff>